<commit_message>
Empty spiders list page is created
</commit_message>
<xml_diff>
--- a/Documentation/Talents.xlsx
+++ b/Documentation/Talents.xlsx
@@ -4452,8 +4452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>